<commit_message>
added blocking to qPCR stats, did nothing lol
</commit_message>
<xml_diff>
--- a/qPCR/qPCR summary.xlsx
+++ b/qPCR/qPCR summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/spet4768_ox_ac_uk/Documents/Desktop/Results/OPLA LF vs HF/qPCR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/spet4768_ox_ac_uk/Documents/Desktop/Results/OPLA-LF-vs-HF/qPCR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="8_{F16A8A5A-DC45-4C93-A9B5-58D6DCDD588F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCC28894-A39B-4964-8BCD-A2D282D57E02}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="8_{F16A8A5A-DC45-4C93-A9B5-58D6DCDD588F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BE718FA-AE5C-44D0-B7E4-0490494FDA06}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E5F79E3C-BF5D-471F-8E2D-88BDCC131A76}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>SampleID</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>ATG5</t>
+  </si>
+  <si>
+    <t>Round</t>
   </si>
 </sst>
 </file>
@@ -1793,8 +1796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B526FC81-1477-4E5A-88EB-B18BFF23CD3D}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3155,361 +3158,391 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E9290C-4E2F-49AD-95C5-1427DAC8DC7E}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.87267324574861538</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.79147248534563575</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.0636145135815316</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.86774473569000021</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.9565149525367711</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1.0661146345642356</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>1.0200661067020367</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>1.1887787124726923</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.8847180594768923</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.7894884995102297</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>1.091608868933988</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>1.0380009549621076</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>1.3154741001860544</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.73313093120957573</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.95196662905235152</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1.1909283880207873</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.95055705878894958</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1.1194953439739859</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.9637239880180194</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>1.2747913462461866</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>1.6003542377776734</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>1.3655935921700348</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2.0941779385000996</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1.0024151911785215</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1.3681371181743123</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.4813797679933243</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1.3521208425756968</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1.5641339782961592</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.4512908951696328</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1.4434977385222481</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
         <v>200</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.67140694679338198</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.82069043667730091</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.97349239935358456</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.83476343995187607</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.95744292225969596</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1.0485321301540687</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.81853930072517322</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>1.1059306295865605</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>0.8161897493071093</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>0.85876461503412271</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
         <v>200</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.73072214604468633</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.72253790444684596</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.87194070402938839</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.51285100802607231</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.70052388844002034</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.87845511836087642</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.59029022096405481</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.82373672231836326</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.65882154682453398</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>0.93327764499048671</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
         <v>200</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>1.2549941578567907</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1.2353423164636377</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1.2946752189427699</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1.0085694462475687</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1.3517398138302354</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1.6520530177707569</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1.0706211984361591</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>1.5344217984696238</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>1.3022810195209993</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>1.1580530100252919</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>800</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.76907488146245473</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.80508135413331272</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1.0281361611857054</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.77862111201183837</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.94346298704160214</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>1.0407523201054145</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.88090686160816511</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>1.0511870459145733</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.8203168721906362</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>0.7086619077042452</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
         <v>800</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>1.048157672438442</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1.1242409020849611</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1.4048958538756686</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>0.82983727874762869</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1.081651724835988</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>1.4892601027231427</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.93092566315538194</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>1.02791308691966</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.97873053077804084</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>1.327635378922329</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
         <v>800</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.66550027906175668</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1.0440569745318433</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1.2461531384657656</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>0.74116397999638695</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>1.1473323961055899</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1.6050497670190496</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.96647866559947937</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1.0231966718030725</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1.037355679252703</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>0.97094351041632976</v>
       </c>
     </row>

</xml_diff>